<commit_message>
Update YTS Movie Notifyer workflow to YTS Movie Scraper
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -468,7 +468,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -480,17 +480,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Monkey Man</t>
+          <t>Arthur the King</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>Adventure</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -502,34 +502,34 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Arthur the King</t>
+          <t>[FR] Infested</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Adventure</t>
+          <t>Horror</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>7.1</t>
+          <t>6.7</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>2023</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Problemista</t>
+          <t>Monkey Man</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Comedy</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -539,14 +539,14 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2024</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Rebel Moon - Part Two: The Scargiver</t>
+          <t>The Old Oak</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -556,19 +556,19 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>5.2</t>
+          <t>7.1</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>2023</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>[FR] The Three Musketeers - Part II: Milady</t>
+          <t>The Mitchells vs. the Machines</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -578,19 +578,19 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>6.5</t>
+          <t>7.6</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2021</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>The Old Oak</t>
+          <t>The Commuter</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -600,19 +600,19 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>7.1</t>
+          <t>6.3</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2018</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>The Little Things</t>
+          <t>Justice League: Crisis on Infinite Earths - Part Two</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -622,19 +622,19 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>6.3</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2021</t>
+          <t>2024</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Good Burger 2</t>
+          <t>Alice Through the Looking Glass</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -644,19 +644,19 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>5.3</t>
+          <t>6.2</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2016</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>The Pod Generation</t>
+          <t>The Little Things</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -666,19 +666,19 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>6.3</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2021</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Justice League: Crisis on Infinite Earths - Part Two</t>
+          <t>Good Burger 2</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -688,19 +688,19 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>6.1</t>
+          <t>5.3</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>2023</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Gods of Egypt</t>
+          <t>The Pod Generation</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -710,51 +710,51 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>5.4</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2023</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Mean Girls</t>
+          <t>Gods of Egypt</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Comedy</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>5.4</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>2016</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Drive-Away Dolls</t>
+          <t>Mean Girls</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>Comedy</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>5.5</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -766,7 +766,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>The Channel</t>
+          <t>Drive-Away Dolls</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -776,29 +776,29 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>5.5</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2024</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Late Night with the Devil</t>
+          <t>Problemista</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Horror</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -810,17 +810,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>One Life</t>
+          <t>The Channel</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Biography</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>7.6</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -832,17 +832,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Immaculate</t>
+          <t>Rebel Moon - Part Two: The Scargiver</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Horror</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -854,17 +854,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>The Bricklayer</t>
+          <t>Late Night with the Devil</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>Horror</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>5.1</t>
+          <t>7.1</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -876,7 +876,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Dune: Part Two</t>
+          <t>One Life</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -886,12 +886,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>8.7</t>
+          <t>7.6</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>2023</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add movie scraping functionality and update report with new data
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -458,17 +458,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Borderlands</t>
+          <t>Don't Move</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>Horror</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>4.4</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -480,7 +480,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Trap</t>
+          <t>Joker: Folie à Deux</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -490,7 +490,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5.3</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -502,7 +502,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>The Deliverance</t>
+          <t>Terrifier 3</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -512,7 +512,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>5.1</t>
+          <t>6.7</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -524,17 +524,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>The Heiress and the Handyman</t>
+          <t>Am I Racist?</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Romance</t>
+          <t>Comedy</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -546,17 +546,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Sister Wife Murder</t>
+          <t>[FR] Family Pack</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Crime</t>
+          <t>Adventure</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>6.7</t>
+          <t>5.4</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -568,17 +568,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Toby Keith: American Icon</t>
+          <t>Transformers One</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Music</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>7.7</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -590,17 +590,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>[TE] Kalki 2898 AD</t>
+          <t>Carved</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>Comedy</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -612,17 +612,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>The Supremes at Earl's All-You-Can-Eat</t>
+          <t>Bagman</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Comedy</t>
+          <t>Horror</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -634,17 +634,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>The Supremes at Earl's All-You-Can-Eat</t>
+          <t>Die Alone</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Comedy</t>
+          <t>Horror</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -656,73 +656,73 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Doctor Jekyll</t>
+          <t>Sweet Bobby: My Catfish Nightmare</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Drama</t>
+          <t>Documentary</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>6.2</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2024</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>[GU] Trisha on the Rocks</t>
+          <t>Death Becomes Her</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Comedy</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>5.4</t>
+          <t>6.7</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>1992</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>[ZH] 18×2 Beyond Youthful Days</t>
+          <t>Armageddon Time</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Drama</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>6.5</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>2022</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>High Noon</t>
+          <t>Cowboys &amp; Aliens</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -732,46 +732,46 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>7.9</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>1952</t>
+          <t>2011</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>WarGames</t>
+          <t>Oddity</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>Horror</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>7.1</t>
+          <t>6.7</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1983</t>
+          <t>2024</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>The Wolfman</t>
+          <t>Cuckoo</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>Horror</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -781,14 +781,14 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2010</t>
+          <t>2024</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Blue Velvet</t>
+          <t>Friday the 13th</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -798,41 +798,41 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>7.7</t>
+          <t>5.5</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1986</t>
+          <t>2009</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Species II</t>
+          <t>Slingshot</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>Sci-Fi</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>1998</t>
+          <t>2024</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Kindergarten Cop</t>
+          <t>A Nightmare on Elm Street</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -842,19 +842,19 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>6.2</t>
+          <t>7.4</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1990</t>
+          <t>1984</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>[FR] Mayhem!</t>
+          <t>You're Next</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -864,19 +864,19 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>6.3</t>
+          <t>6.6</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2011</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>A Christmas Story</t>
+          <t>Night Train</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -886,12 +886,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>7.9</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1983</t>
+          <t>2023</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update report with new movie data and add DataFrame section
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -458,17 +458,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Don't Move</t>
+          <t>Mary</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Horror</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>5.9</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -480,17 +480,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Joker: Folie à Deux</t>
+          <t>Red One</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Crime</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>5.3</t>
+          <t>6.7</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -502,7 +502,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Terrifier 3</t>
+          <t>Heretic</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -512,7 +512,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>6.7</t>
+          <t>7.1</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -524,17 +524,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Am I Racist?</t>
+          <t>Venom: The Last Dance</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Comedy</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6.1</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -546,17 +546,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>[FR] Family Pack</t>
+          <t>[TA] Thangalaan</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Adventure</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>5.4</t>
+          <t>6.9</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -568,17 +568,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Transformers One</t>
+          <t>The Best Christmas Pageant Ever</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>Adventure</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>7.7</t>
+          <t>7</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -590,17 +590,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Carved</t>
+          <t>Juror #2</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Comedy</t>
+          <t>Crime</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>4.4</t>
+          <t>7.1</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -612,17 +612,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Bagman</t>
+          <t>That Christmas</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Horror</t>
+          <t>Adventure</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>6.8</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -634,17 +634,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Die Alone</t>
+          <t>Holiday Touchdown: A Chiefs Love Story</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Horror</t>
+          <t>Comedy</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -656,17 +656,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Sweet Bobby: My Catfish Nightmare</t>
+          <t>[HI] Sikandar Ka Muqaddar</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Documentary</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>6.2</t>
+          <t>6.1</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -678,51 +678,51 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Death Becomes Her</t>
+          <t>[TE] Lucky Baskhar</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>Crime</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>6.7</t>
+          <t>8.1</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1992</t>
+          <t>2024</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Armageddon Time</t>
+          <t>[FR] The Seed of the Sacred Fig</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>Crime</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>6.5</t>
+          <t>7.6</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2024</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Cowboys &amp; Aliens</t>
+          <t>The Convert</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -732,95 +732,95 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2011</t>
+          <t>2023</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Oddity</t>
+          <t>[KO] Project Silence</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Horror</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>6.7</t>
+          <t>5.5</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>2023</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Cuckoo</t>
+          <t>David Attenborough: A Life on Our Planet</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Horror</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>5.8</t>
+          <t>8.9</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>2020</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Friday the 13th</t>
+          <t>The Substance</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>Drama</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>5.5</t>
+          <t>7.4</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2009</t>
+          <t>2024</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Slingshot</t>
+          <t>[HI] Jigra</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Sci-Fi</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -832,7 +832,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>A Nightmare on Elm Street</t>
+          <t>[FR] Cat and Dog</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -842,41 +842,41 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>7.4</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1984</t>
+          <t>2024</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>You're Next</t>
+          <t>Conclave</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>Drama</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>6.6</t>
+          <t>7.4</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2011</t>
+          <t>2024</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Night Train</t>
+          <t>Freud's Last Session</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -886,7 +886,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>6.1</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">

</xml_diff>

<commit_message>
Add DataFrame section to report and update movie data
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Mary</t>
+          <t>The Lord of the Rings: The War of the Rohirrim</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -468,7 +468,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>5.2</t>
+          <t>6.6</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -480,7 +480,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Red One</t>
+          <t>Gladiator II</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -490,7 +490,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>6.7</t>
+          <t>6.8</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -502,17 +502,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Heretic</t>
+          <t>The Order</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Horror</t>
+          <t>Crime</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>7.1</t>
+          <t>7</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -524,17 +524,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Venom: The Last Dance</t>
+          <t>The Six Triple Eight</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>Drama</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>6.1</t>
+          <t>6.5</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -546,17 +546,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>[TA] Thangalaan</t>
+          <t>Bird</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>Drama</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>6.9</t>
+          <t>7.2</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -568,12 +568,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>The Best Christmas Pageant Ever</t>
+          <t>Small Things Like These</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Adventure</t>
+          <t>Drama</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -590,17 +590,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Juror #2</t>
+          <t>Anora</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Crime</t>
+          <t>Comedy</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>7.1</t>
+          <t>8</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -612,17 +612,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>That Christmas</t>
+          <t>Dirty Angels</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Adventure</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>6.8</t>
+          <t>4.1</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -634,17 +634,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Holiday Touchdown: A Chiefs Love Story</t>
+          <t>Omni Loop</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Comedy</t>
+          <t>Drama</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>5.5</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -656,7 +656,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>[HI] Sikandar Ka Muqaddar</t>
+          <t>DragonHeart</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -666,29 +666,29 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>6.1</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>1996</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>[TE] Lucky Baskhar</t>
+          <t>Megalopolis</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Crime</t>
+          <t>Drama</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -700,29 +700,29 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>[FR] The Seed of the Sacred Fig</t>
+          <t>Hush</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Crime</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>7.6</t>
+          <t>6.6</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>2016</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>The Convert</t>
+          <t>Candyman</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -732,19 +732,19 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>6.7</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>1992</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>[KO] Project Silence</t>
+          <t>Teenage Mutant Ninja Turtles: Out of the Shadows</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -754,19 +754,19 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>5.5</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2016</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>David Attenborough: A Life on Our Planet</t>
+          <t>Demolition Man</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -776,41 +776,41 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>8.9</t>
+          <t>6.7</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>1993</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>The Substance</t>
+          <t>[ES] The Settlers</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Drama</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>7.4</t>
+          <t>6.9</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>2023</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>[HI] Jigra</t>
+          <t>Twin Peaks: Fire Walk with Me</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -820,19 +820,19 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>1992</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>[FR] Cat and Dog</t>
+          <t>The Last House on the Left</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -842,41 +842,41 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>5.2</t>
+          <t>6.5</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>2009</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Conclave</t>
+          <t>Ted</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Drama</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>7.4</t>
+          <t>6.9</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>2012</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Freud's Last Session</t>
+          <t>Starve Acre</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -886,7 +886,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>6.1</t>
+          <t>5.4</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">

</xml_diff>

<commit_message>
Add DataFrame section to report with new movie entries
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -458,17 +458,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>The Lord of the Rings: The War of the Rohirrim</t>
+          <t>The Order</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>Crime</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>6.6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -480,17 +480,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Gladiator II</t>
+          <t>Bird</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>Drama</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>6.8</t>
+          <t>7.2</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -502,17 +502,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>The Order</t>
+          <t>The Lord of the Rings: The War of the Rohirrim</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Crime</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6.6</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -524,17 +524,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Bird</t>
+          <t>Gladiator II</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Drama</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>6.8</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -546,39 +546,39 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Anora</t>
+          <t>[DA] The Promised Land</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Comedy</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>7.7</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>2023</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Dirty Angels</t>
+          <t>The Six Triple Eight</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>Drama</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>4.1</t>
+          <t>6.5</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -590,7 +590,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>[DA] The Promised Land</t>
+          <t>DragonHeart</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -600,19 +600,19 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>7.7</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>1996</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>The Six Triple Eight</t>
+          <t>Megalopolis</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -622,7 +622,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>6.5</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -634,7 +634,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>DragonHeart</t>
+          <t>Hush</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -644,41 +644,41 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>6.6</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>1996</t>
+          <t>2016</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Megalopolis</t>
+          <t>Candyman</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Drama</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>6.7</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>1992</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Hush</t>
+          <t>Teenage Mutant Ninja Turtles: Out of the Shadows</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -688,7 +688,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>6.6</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -700,7 +700,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Candyman</t>
+          <t>Demolition Man</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -715,14 +715,14 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1992</t>
+          <t>1993</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Teenage Mutant Ninja Turtles: Out of the Shadows</t>
+          <t>[ES] The Settlers</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -732,19 +732,19 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>5.9</t>
+          <t>6.9</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2023</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Demolition Man</t>
+          <t>Twin Peaks: Fire Walk with Me</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -754,19 +754,19 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>6.7</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>1993</t>
+          <t>1992</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>[ES] The Settlers</t>
+          <t>The Last House on the Left</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -776,19 +776,19 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>6.9</t>
+          <t>6.5</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2009</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Twin Peaks: Fire Walk with Me</t>
+          <t>Ted</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -798,19 +798,19 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>6.9</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1992</t>
+          <t>2012</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>The Last House on the Left</t>
+          <t>Starve Acre</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -820,19 +820,19 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>6.5</t>
+          <t>5.4</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2009</t>
+          <t>2023</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Ted</t>
+          <t>The Forge</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -842,19 +842,19 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>6.9</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2012</t>
+          <t>2024</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Starve Acre</t>
+          <t>Sideways</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -864,29 +864,29 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>5.4</t>
+          <t>7.5</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2004</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>The Forge</t>
+          <t>[TH] How to Make Millions Before Grandma Dies</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>Comedy</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>8</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">

</xml_diff>

<commit_message>
Update report and code with new movie entries and DataFrame section
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -458,12 +458,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Wallace &amp; Gromit: Vengeance Most Fowl</t>
+          <t>Wicked</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Adventure</t>
+          <t>Fantasy</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -480,17 +480,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>The Order</t>
+          <t>Wallace &amp; Gromit: Vengeance Most Fowl</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Crime</t>
+          <t>Adventure</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -502,17 +502,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bird</t>
+          <t>The Lord of the Rings: The War of the Rohirrim</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Drama</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>6.6</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -524,7 +524,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>The Lord of the Rings: The War of the Rohirrim</t>
+          <t>Gladiator II</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -534,7 +534,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>6.6</t>
+          <t>6.8</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -546,7 +546,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Gladiator II</t>
+          <t>Red One</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -556,7 +556,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>6.8</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -568,7 +568,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Red One</t>
+          <t>Venom: The Last Dance</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -578,7 +578,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -590,17 +590,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Venom: The Last Dance</t>
+          <t>Joker: Folie à Deux</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>Crime</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -612,17 +612,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Joker: Folie à Deux</t>
+          <t>Beetlejuice Beetlejuice</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Crime</t>
+          <t>Comedy</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>5.2</t>
+          <t>6.7</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -634,7 +634,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Beetlejuice Beetlejuice</t>
+          <t>A Different Man</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -644,7 +644,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>6.7</t>
+          <t>7</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -656,17 +656,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>A Different Man</t>
+          <t>[HI] Yodha</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Comedy</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -678,7 +678,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>[HI] Yodha</t>
+          <t>[HI] Singham Again</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -688,7 +688,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>5.3</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -700,17 +700,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>[HI] Singham Again</t>
+          <t>Saturday Night</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>Biography</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>5.3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -722,29 +722,29 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Saturday Night</t>
+          <t>Mr. Monk's Last Case: A Monk Movie</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Biography</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6.7</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>2023</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Mr. Monk's Last Case: A Monk Movie</t>
+          <t>The Outrun</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -754,29 +754,29 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>6.7</t>
+          <t>6.9</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2024</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>The Outrun</t>
+          <t>The Order</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>Crime</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>6.9</t>
+          <t>7</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -788,110 +788,110 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>[DA] The Promised Land</t>
+          <t>Bird</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>Drama</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>7.7</t>
+          <t>7.2</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2024</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>The Six Triple Eight</t>
+          <t>[DA] The Promised Land</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Drama</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>6.5</t>
+          <t>7.7</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>2023</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>DragonHeart</t>
+          <t>The Six Triple Eight</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>Drama</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>6.5</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>1996</t>
+          <t>2024</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Megalopolis</t>
+          <t>DragonHeart</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Drama</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>1996</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Hush</t>
+          <t>Megalopolis</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>Drama</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>6.6</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2024</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update movie entries and DataFrame in report and code notebook
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -458,17 +458,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Wicked</t>
+          <t>A Real Pain</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Fantasy</t>
+          <t>Comedy</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>7.4</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -480,12 +480,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Wallace &amp; Gromit: Vengeance Most Fowl</t>
+          <t>Wicked</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Adventure</t>
+          <t>Fantasy</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -502,7 +502,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>The Lord of the Rings: The War of the Rohirrim</t>
+          <t>Armor</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -512,7 +512,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>6.6</t>
+          <t>3.5</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -524,17 +524,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Gladiator II</t>
+          <t>A Different Man</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>Comedy</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>6.8</t>
+          <t>7</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -546,7 +546,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Red One</t>
+          <t>[HI] Yodha</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -556,7 +556,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -568,7 +568,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Venom: The Last Dance</t>
+          <t>[HI] Singham Again</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -578,7 +578,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5.3</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -590,17 +590,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Joker: Folie à Deux</t>
+          <t>Saturday Night</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Crime</t>
+          <t>Biography</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>5.2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -612,12 +612,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Beetlejuice Beetlejuice</t>
+          <t>Mr. Monk's Last Case: A Monk Movie</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Comedy</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -627,24 +627,24 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>2023</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>A Different Man</t>
+          <t>The Outrun</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Comedy</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6.9</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -656,17 +656,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>[HI] Yodha</t>
+          <t>Wallace &amp; Gromit: Vengeance Most Fowl</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>Adventure</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>8</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -678,17 +678,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>[HI] Singham Again</t>
+          <t>The Order</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Action</t>
+          <t>Crime</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>5.3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -700,17 +700,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Saturday Night</t>
+          <t>Bird</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Biography</t>
+          <t>Drama</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>7.2</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -722,7 +722,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Mr. Monk's Last Case: A Monk Movie</t>
+          <t>The Lord of the Rings: The War of the Rohirrim</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -732,19 +732,19 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>6.7</t>
+          <t>6.6</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2024</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>The Outrun</t>
+          <t>[DA] The Promised Land</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -754,29 +754,29 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>6.9</t>
+          <t>7.7</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>2023</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>The Order</t>
+          <t>The Six Triple Eight</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Crime</t>
+          <t>Drama</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6.5</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -788,17 +788,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Bird</t>
+          <t>Gladiator II</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Drama</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>6.8</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -810,7 +810,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>[DA] The Promised Land</t>
+          <t>DragonHeart</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -820,19 +820,19 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>7.7</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>1996</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>The Six Triple Eight</t>
+          <t>Megalopolis</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -842,7 +842,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>6.5</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -854,7 +854,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>DragonHeart</t>
+          <t>Hush</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -864,34 +864,34 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>6.6</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>1996</t>
+          <t>2016</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Megalopolis</t>
+          <t>Candyman</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Drama</t>
+          <t>Action</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>6.7</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2024</t>
+          <t>1992</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update movie ratings and add new entries in report and DataFrame
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -468,7 +468,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>7.4</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -490,7 +490,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>7.9</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">

</xml_diff>